<commit_message>
feat update otdr COllo
w
</commit_message>
<xml_diff>
--- a/cypress/downloads/test-StipinputNewBuildMacroresults.xlsx
+++ b/cypress/downloads/test-StipinputNewBuildMacroresults.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,6 +412,9 @@
       <c r="C1" t="str">
         <v>timeStamp</v>
       </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -421,12 +424,34 @@
         <v>Pass</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-04-23T09:29:09.589Z</v>
+        <v>2025-04-23T16:56:17.282Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>User AM melakukan klik tombol Search di Stip approval</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-04-23T16:56:52.942Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>User AM melakukan klik tombol Search di Stip approval</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-04-23T16:56:53.051Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>